<commit_message>
Update E9 HR Data - Dynamic Chart Labels.xlsx
</commit_message>
<xml_diff>
--- a/Exercise Files/Exercise 9/E9 HR Data - Dynamic Chart Labels.xlsx
+++ b/Exercise Files/Exercise 9/E9 HR Data - Dynamic Chart Labels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f21e54c367d3358c/Documents/01 Work Files/05 SSIT/Online Courses/Advanced PivotTables/Exercise Files/Exercise 9/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wayvy Technologies\Documents\GitHub\PivotTables\Exercise Files\Exercise 9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="8_{FD91D03E-95D7-47CE-9451-B718983BE210}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B2889575-8D98-4275-8AAF-A087A64A7629}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACE790E-3CFC-4995-80A4-0616129B7BCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{960E11C6-F8C0-4296-BE1C-66F0D68FFF3E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{960E11C6-F8C0-4296-BE1C-66F0D68FFF3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Employee Info" sheetId="1" r:id="rId1"/>
@@ -23,14 +23,14 @@
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Employee Info'!$A$1:$C$100</definedName>
-    <definedName name="_xlcn.WorksheetConnection_HRDataConsolidating.xlsxTable1" hidden="1">'Employee Info'!$A$1:$C$100</definedName>
-    <definedName name="_xlcn.WorksheetConnection_HRDataConsolidating.xlsxTable2" hidden="1">'[1]Department Info'!$A$1:$A$100</definedName>
-    <definedName name="_xlcn.WorksheetConnection_HRDataConsolidating.xlsxTable3" hidden="1">'[2]Job Info'!$A$1:$A$100</definedName>
+    <definedName name="_xlcn.WorksheetConnection_HRDataConsolidating.xlsxTable11" hidden="1">'Employee Info'!$A$1:$C$100</definedName>
+    <definedName name="_xlcn.WorksheetConnection_HRDataConsolidating.xlsxTable21" hidden="1">'[1]Department Info'!$A$1:$A$100</definedName>
+    <definedName name="_xlcn.WorksheetConnection_HRDataConsolidating.xlsxTable31" hidden="1">'[2]Job Info'!$A$1:$A$100</definedName>
     <definedName name="Slicer_Job_Type">#N/A</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
+    <pivotCache cacheId="13" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -84,7 +84,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Table1" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_HRDataConsolidating.xlsxTable1"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_HRDataConsolidating.xlsxTable11"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -93,7 +93,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Table2">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_HRDataConsolidating.xlsxTable2"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_HRDataConsolidating.xlsxTable21"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -102,7 +102,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Table3">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_HRDataConsolidating.xlsxTable3"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_HRDataConsolidating.xlsxTable31"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -576,7 +576,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -584,7 +584,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
@@ -1860,7 +1859,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Department Info"/>
@@ -1873,7 +1872,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Job Info"/>
@@ -3136,7 +3135,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FE3D0495-A9B3-4C5A-ADEE-A30D98D35ADE}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FE3D0495-A9B3-4C5A-ADEE-A30D98D35ADE}" name="PivotTable4" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:B11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField showAll="0"/>
@@ -3377,9 +3376,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3417,7 +3416,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3523,7 +3522,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3665,7 +3664,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3675,23 +3674,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91CF34E-7D4C-4202-8C48-E09665776E8A}">
   <dimension ref="A1:I100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="4" width="22.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.88671875" customWidth="1"/>
-    <col min="6" max="6" width="24.109375" style="1" customWidth="1"/>
-    <col min="7" max="8" width="20.21875" customWidth="1"/>
-    <col min="9" max="9" width="18.21875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" style="1" customWidth="1"/>
+    <col min="7" max="8" width="20.28515625" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3720,7 +3719,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2100</v>
       </c>
@@ -3749,7 +3748,7 @@
         <v>40445</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2101</v>
       </c>
@@ -3778,7 +3777,7 @@
         <v>42551</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2102</v>
       </c>
@@ -3807,7 +3806,7 @@
         <v>43376</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2103</v>
       </c>
@@ -3836,7 +3835,7 @@
         <v>43168</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2104</v>
       </c>
@@ -3865,7 +3864,7 @@
         <v>40164</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2105</v>
       </c>
@@ -3894,7 +3893,7 @@
         <v>40511</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2106</v>
       </c>
@@ -3923,7 +3922,7 @@
         <v>43915</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2107</v>
       </c>
@@ -3952,7 +3951,7 @@
         <v>38555</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2108</v>
       </c>
@@ -3981,7 +3980,7 @@
         <v>42421</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2109</v>
       </c>
@@ -4010,7 +4009,7 @@
         <v>43151</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2110</v>
       </c>
@@ -4039,7 +4038,7 @@
         <v>42809</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2111</v>
       </c>
@@ -4068,7 +4067,7 @@
         <v>40378</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2112</v>
       </c>
@@ -4097,7 +4096,7 @@
         <v>40976</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2113</v>
       </c>
@@ -4126,7 +4125,7 @@
         <v>36845</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2114</v>
       </c>
@@ -4155,7 +4154,7 @@
         <v>42217</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2115</v>
       </c>
@@ -4184,7 +4183,7 @@
         <v>41198</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2116</v>
       </c>
@@ -4213,7 +4212,7 @@
         <v>36704</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2117</v>
       </c>
@@ -4242,7 +4241,7 @@
         <v>42895</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2118</v>
       </c>
@@ -4271,7 +4270,7 @@
         <v>41286</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2119</v>
       </c>
@@ -4300,7 +4299,7 @@
         <v>39319</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2120</v>
       </c>
@@ -4329,7 +4328,7 @@
         <v>40839</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2121</v>
       </c>
@@ -4358,7 +4357,7 @@
         <v>36754</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2122</v>
       </c>
@@ -4387,7 +4386,7 @@
         <v>38170</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2123</v>
       </c>
@@ -4416,7 +4415,7 @@
         <v>39164</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2124</v>
       </c>
@@ -4445,7 +4444,7 @@
         <v>42219</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2125</v>
       </c>
@@ -4474,7 +4473,7 @@
         <v>40652</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2126</v>
       </c>
@@ -4503,7 +4502,7 @@
         <v>41065</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2127</v>
       </c>
@@ -4532,7 +4531,7 @@
         <v>39692</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2128</v>
       </c>
@@ -4561,7 +4560,7 @@
         <v>42030</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2129</v>
       </c>
@@ -4590,7 +4589,7 @@
         <v>39499</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2130</v>
       </c>
@@ -4619,7 +4618,7 @@
         <v>43695</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2131</v>
       </c>
@@ -4648,7 +4647,7 @@
         <v>42324</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2132</v>
       </c>
@@ -4677,7 +4676,7 @@
         <v>36600</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2133</v>
       </c>
@@ -4706,7 +4705,7 @@
         <v>39803</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2134</v>
       </c>
@@ -4735,7 +4734,7 @@
         <v>40249</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2135</v>
       </c>
@@ -4764,7 +4763,7 @@
         <v>38971</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2136</v>
       </c>
@@ -4793,7 +4792,7 @@
         <v>40276</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2137</v>
       </c>
@@ -4822,7 +4821,7 @@
         <v>38241</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2138</v>
       </c>
@@ -4851,7 +4850,7 @@
         <v>40684</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2139</v>
       </c>
@@ -4880,7 +4879,7 @@
         <v>39996</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2140</v>
       </c>
@@ -4909,7 +4908,7 @@
         <v>37411</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2141</v>
       </c>
@@ -4938,7 +4937,7 @@
         <v>43850</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2142</v>
       </c>
@@ -4967,7 +4966,7 @@
         <v>43170</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2143</v>
       </c>
@@ -4996,7 +4995,7 @@
         <v>37292</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2144</v>
       </c>
@@ -5025,7 +5024,7 @@
         <v>37609</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2145</v>
       </c>
@@ -5054,7 +5053,7 @@
         <v>37094</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2146</v>
       </c>
@@ -5083,7 +5082,7 @@
         <v>42118</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2147</v>
       </c>
@@ -5112,7 +5111,7 @@
         <v>41517</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2148</v>
       </c>
@@ -5141,7 +5140,7 @@
         <v>38742</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2149</v>
       </c>
@@ -5170,7 +5169,7 @@
         <v>40047</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2150</v>
       </c>
@@ -5199,7 +5198,7 @@
         <v>39802</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2151</v>
       </c>
@@ -5228,7 +5227,7 @@
         <v>39616</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2152</v>
       </c>
@@ -5257,7 +5256,7 @@
         <v>41686</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2153</v>
       </c>
@@ -5286,7 +5285,7 @@
         <v>39019</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2154</v>
       </c>
@@ -5315,7 +5314,7 @@
         <v>41028</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2155</v>
       </c>
@@ -5344,7 +5343,7 @@
         <v>39768</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2156</v>
       </c>
@@ -5373,7 +5372,7 @@
         <v>41153</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2157</v>
       </c>
@@ -5402,7 +5401,7 @@
         <v>36847</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2158</v>
       </c>
@@ -5431,7 +5430,7 @@
         <v>37105</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2159</v>
       </c>
@@ -5460,7 +5459,7 @@
         <v>39744</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2160</v>
       </c>
@@ -5489,7 +5488,7 @@
         <v>43167</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2161</v>
       </c>
@@ -5518,7 +5517,7 @@
         <v>38401</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2162</v>
       </c>
@@ -5547,7 +5546,7 @@
         <v>37956</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2163</v>
       </c>
@@ -5576,7 +5575,7 @@
         <v>43907</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2164</v>
       </c>
@@ -5605,7 +5604,7 @@
         <v>43669</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2165</v>
       </c>
@@ -5634,7 +5633,7 @@
         <v>39740</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2166</v>
       </c>
@@ -5663,7 +5662,7 @@
         <v>40408</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2167</v>
       </c>
@@ -5692,7 +5691,7 @@
         <v>38822</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2168</v>
       </c>
@@ -5721,7 +5720,7 @@
         <v>40083</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2169</v>
       </c>
@@ -5750,7 +5749,7 @@
         <v>41579</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2170</v>
       </c>
@@ -5779,7 +5778,7 @@
         <v>43027</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2171</v>
       </c>
@@ -5808,7 +5807,7 @@
         <v>41582</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2172</v>
       </c>
@@ -5837,7 +5836,7 @@
         <v>36663</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2173</v>
       </c>
@@ -5866,7 +5865,7 @@
         <v>37526</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2174</v>
       </c>
@@ -5895,7 +5894,7 @@
         <v>41710</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>2175</v>
       </c>
@@ -5924,7 +5923,7 @@
         <v>40274</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2176</v>
       </c>
@@ -5953,7 +5952,7 @@
         <v>40107</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2177</v>
       </c>
@@ -5982,7 +5981,7 @@
         <v>39142</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2178</v>
       </c>
@@ -6011,7 +6010,7 @@
         <v>39165</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>2179</v>
       </c>
@@ -6040,7 +6039,7 @@
         <v>42462</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>2180</v>
       </c>
@@ -6069,7 +6068,7 @@
         <v>41654</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>2181</v>
       </c>
@@ -6098,7 +6097,7 @@
         <v>43128</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2182</v>
       </c>
@@ -6127,7 +6126,7 @@
         <v>43381</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>2183</v>
       </c>
@@ -6156,7 +6155,7 @@
         <v>41676</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>2184</v>
       </c>
@@ -6185,7 +6184,7 @@
         <v>36651</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>2185</v>
       </c>
@@ -6214,7 +6213,7 @@
         <v>42526</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>2186</v>
       </c>
@@ -6243,7 +6242,7 @@
         <v>38565</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>2187</v>
       </c>
@@ -6272,7 +6271,7 @@
         <v>37518</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>2188</v>
       </c>
@@ -6301,7 +6300,7 @@
         <v>39656</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>2189</v>
       </c>
@@ -6330,7 +6329,7 @@
         <v>41701</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>2190</v>
       </c>
@@ -6359,7 +6358,7 @@
         <v>42528</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>2191</v>
       </c>
@@ -6388,7 +6387,7 @@
         <v>38499</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>2192</v>
       </c>
@@ -6417,7 +6416,7 @@
         <v>43550</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>2193</v>
       </c>
@@ -6446,7 +6445,7 @@
         <v>38384</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>2194</v>
       </c>
@@ -6475,7 +6474,7 @@
         <v>42668</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>2195</v>
       </c>
@@ -6504,7 +6503,7 @@
         <v>43124</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>2196</v>
       </c>
@@ -6533,7 +6532,7 @@
         <v>37442</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>2197</v>
       </c>
@@ -6562,7 +6561,7 @@
         <v>38690</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>2198</v>
       </c>
@@ -6607,13 +6606,13 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -6621,7 +6620,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>125</v>
       </c>
@@ -6629,67 +6628,67 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11">
         <v>99</v>
       </c>
     </row>
@@ -6710,35 +6709,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2131E3D1-EA48-46F3-AD8B-FBF57C58DBB9}">
   <dimension ref="A2:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="12" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+    <row r="12" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
+    <row r="13" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="16" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
+    <row r="16" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>133</v>
       </c>
     </row>

</xml_diff>